<commit_message>
ddd Signed-off-by: peixere <peixere@qq.com>
</commit_message>
<xml_diff>
--- a/cnplay/doc/抵质押物品导入模版.xlsx
+++ b/cnplay/doc/抵质押物品导入模版.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -54,7 +54,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>98611120170160211-01</t>
+    <t>98611120170160211-01333</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,17 +429,17 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="1" max="1" width="24.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -528,7 +528,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -542,7 +542,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>